<commit_message>
A couple of experiments to see the effect of TPR only.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Experiment description</t>
   </si>
@@ -60,6 +60,38 @@
   </si>
   <si>
     <t>EXP2.txt</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Done!</t>
+  </si>
+  <si>
+    <t>Just TPR no LSTM in 
+phrase embedding layer</t>
+  </si>
+  <si>
+    <t>DLT1 / 3</t>
+  </si>
+  <si>
+    <t>EXP3.txt</t>
+  </si>
+  <si>
+    <t>Just LSTM no TPR in 
+phrase embedding layer</t>
+  </si>
+  <si>
+    <t>EXP4.txt</t>
+  </si>
+  <si>
+    <t>pane number in tmux</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justTPR True --batch_size 60 --run_id 0 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP3.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justLSTM True --batch_size 60 --run_id 1 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP4.txt</t>
   </si>
 </sst>
 </file>
@@ -414,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,9 +458,10 @@
     <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +477,14 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -461,8 +500,11 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -476,6 +518,49 @@
         <v>12</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kicked off 5 experiments on DLT1!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Experiment description</t>
   </si>
@@ -68,30 +68,70 @@
     <t>Done!</t>
   </si>
   <si>
+    <t>DLT1 / 3</t>
+  </si>
+  <si>
+    <t>EXP3.txt</t>
+  </si>
+  <si>
+    <t>EXP4.txt</t>
+  </si>
+  <si>
+    <t>pane number in tmux</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justTPR True --batch_size 60 --run_id 0 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP3.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justLSTM True --batch_size 60 --run_id 1 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP4.txt</t>
+  </si>
+  <si>
     <t>Just TPR no LSTM in 
-phrase embedding layer</t>
-  </si>
-  <si>
-    <t>DLT1 / 3</t>
-  </si>
-  <si>
-    <t>EXP3.txt</t>
+phrase embedding layer 
+batchsize = 60</t>
   </si>
   <si>
     <t>Just LSTM no TPR in 
-phrase embedding layer</t>
-  </si>
-  <si>
-    <t>EXP4.txt</t>
-  </si>
-  <si>
-    <t>pane number in tmux</t>
-  </si>
-  <si>
-    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justTPR True --batch_size 60 --run_id 0 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP3.txt</t>
-  </si>
-  <si>
-    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justLSTM True --batch_size 60 --run_id 1 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP4.txt</t>
+phrase embedding layer 
+batchsize = 60</t>
+  </si>
+  <si>
+    <t>Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justTPR True --batch_size 40 --run_id 2 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP5.txt</t>
+  </si>
+  <si>
+    <t>EXP5.txt</t>
+  </si>
+  <si>
+    <t>DLT1 / 2</t>
+  </si>
+  <si>
+    <t>Just LSTM no TPR in 
+phrase embedding layer 
+batchsize = 40</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR False --justLSTM True --batch_size 40 --run_id 3 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP6.txt</t>
+  </si>
+  <si>
+    <t>EXP6.txt</t>
+  </si>
+  <si>
+    <t>LSTM output concatenated with TPR output in phrase embedding layer. No mixed TPR+LSTM cell for this experiment. 
+batchsize = 40</t>
+  </si>
+  <si>
+    <t>DLT1 / 7</t>
+  </si>
+  <si>
+    <t>EXP7.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --batch_size 40 --run_id 4 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP7.txt</t>
   </si>
 </sst>
 </file>
@@ -446,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -524,18 +564,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -544,24 +584,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kicked off 1 experiments on DLT1 for speed benchmarking!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Experiment description</t>
   </si>
@@ -132,6 +132,19 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --batch_size 40 --run_id 4 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP7.txt</t>
+  </si>
+  <si>
+    <t>Running Original AI2 QA code again for comparison purposes 
+batchsize = 60</t>
+  </si>
+  <si>
+    <t>DLT1 / 6</t>
+  </si>
+  <si>
+    <t>EXP8.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --batch_size 60 --run_id 5 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP8.txt</t>
   </si>
 </sst>
 </file>
@@ -486,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,6 +677,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-run speed benchmarking experiment, it was killed in the morning. Two experiments done. All on DLT1!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Experiment description</t>
   </si>
@@ -136,9 +136,6 @@
   <si>
     <t>Running Original AI2 QA code again for comparison purposes 
 batchsize = 60</t>
-  </si>
-  <si>
-    <t>DLT1 / 6</t>
   </si>
   <si>
     <t>EXP8.txt</t>
@@ -160,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,11 +183,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +509,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,6 +519,7 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -577,123 +585,129 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Collected the experiment results on DLT1!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Experiment description</t>
   </si>
@@ -509,7 +509,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +650,9 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -670,6 +673,9 @@
       <c r="F8" s="3">
         <v>2</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -690,6 +696,9 @@
       <c r="F9" s="3">
         <v>4</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -709,6 +718,9 @@
       </c>
       <c r="F10" s="3">
         <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Experiments excel file with accuracy / F1 / loss info of train / dev set.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Experiment description</t>
   </si>
@@ -144,14 +144,121 @@
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --batch_size 60 --run_id 5 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP8.txt</t>
   </si>
   <si>
-    <t>Done!!</t>
+    <t>EXP9.txt</t>
+  </si>
+  <si>
+    <t>Using new TPR-LSTM cell. 
+batchsize = 40</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell True --batch_size 40 --run_id 6 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP9.txt</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>train set result
+accuracy / F1 / loss</t>
+  </si>
+  <si>
+    <t>dev set result
+accuracy / F1 / loss</t>
+  </si>
+  <si>
+    <t>0.6402 / 0.7882 / 1.773</t>
+  </si>
+  <si>
+    <t>0.5962 / 0.7086 / 3.232</t>
+  </si>
+  <si>
+    <t>33 hr</t>
+  </si>
+  <si>
+    <t>0.6998 / 0.8457 / 1.306</t>
+  </si>
+  <si>
+    <t>0.6212 / 0.7302 / 3.115</t>
+  </si>
+  <si>
+    <t>0.5825 / 0.7238 / 2.268</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>0.5533 / 0.663 / 3.493</t>
+  </si>
+  <si>
+    <t>34 hr</t>
+  </si>
+  <si>
+    <t>0.6507 / 0.7983 / 1.703</t>
+  </si>
+  <si>
+    <t>0.5813 / 0.7008 / 3.435</t>
+  </si>
+  <si>
+    <t>35 hr</t>
+  </si>
+  <si>
+    <t>with different barchsize hyper-params 
+should be fine tuned again otherwise 
+performance degrades.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Feb. 17, 2017</t>
+  </si>
+  <si>
+    <t>0.6715 / 0.8097 / 1.610</t>
+  </si>
+  <si>
+    <t>0.601 / 0.7001 / 3.302</t>
+  </si>
+  <si>
+    <t>39 hr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Always using default TPR params unless 
+mentioned otherwise:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>share_tpr_weights = True
+nSymbols = 100
+dSymbols = 10
+nRoles = 20
+dRoles = 10</t>
+    </r>
+  </si>
+  <si>
+    <t>0.7055 / 0.8412 / 1.318</t>
+  </si>
+  <si>
+    <t>0.6347 / 0.7371 / 3.231</t>
+  </si>
+  <si>
+    <t>30 hr</t>
+  </si>
+  <si>
+    <t>The main reason for this experiment was 
+time benchmarking. This is original AI2 code  without any modifications. I was abale to run this in 15 hr during Christmas holidays when DLT1 machine was not that busy. Please note that computations are usually split between CPU and GPU and when the machine is too busy it makes the total time of experiments much slower which is confirmed by this experiment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +266,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +286,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,19 +301,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,224 +648,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="20.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="38.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>4</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>5</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>6</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
An experiment on DLT2 for time benchmarking compared to DLT1.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Experiment description</t>
   </si>
@@ -252,6 +252,18 @@
   <si>
     <t>The main reason for this experiment was 
 time benchmarking. This is original AI2 code  without any modifications. I was abale to run this in 15 hr during Christmas holidays when DLT1 machine was not that busy. Please note that computations are usually split between CPU and GPU and when the machine is too busy it makes the total time of experiments much slower which is confirmed by this experiment.</t>
+  </si>
+  <si>
+    <t>DLT2 / 6</t>
+  </si>
+  <si>
+    <t>EXP10.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell True --batch_size 40 --run_id 7 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP10.txt</t>
+  </si>
+  <si>
+    <t>The same as experiment in row 11 except here we run it on DLT2 machine for time benchmarking purposes. Currently DLT2 is not as busy as DLT1. This helps because some operations are done on CPU, i.e., DLT1 too busy ==&gt; less CPU cores for my code!</t>
   </si>
 </sst>
 </file>
@@ -648,13 +660,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="7" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +1006,29 @@
         <v>57</v>
       </c>
     </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="6">
+        <v>7</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Experiment for mixed TPR-LSTM cell concluded.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>Experiment description</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>The same as experiment in row 11 except here we run it on DLT2 machine for time benchmarking purposes. Currently DLT2 is not as busy as DLT1. This helps because some operations are done on CPU, i.e., DLT1 too busy ==&gt; less CPU cores for my code!</t>
+  </si>
+  <si>
+    <t>18 hr</t>
+  </si>
+  <si>
+    <t>0.601 / 0.7047 / 3.546</t>
+  </si>
+  <si>
+    <t>0.6777 / 0.8254 / 1.485</t>
   </si>
 </sst>
 </file>
@@ -663,10 +672,8 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="7" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1032,18 @@
       <c r="F12" s="6">
         <v>0</v>
       </c>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="L12" s="6" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Kicked off the experiment in issue #19.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>Experiment description</t>
   </si>
@@ -273,6 +273,30 @@
   </si>
   <si>
     <t>0.6777 / 0.8254 / 1.485</t>
+  </si>
+  <si>
+    <t>TPR cell, batchsize = 40, two times more updates (40,000 instead of 20,000): To see if TPR alone can achieve LSTM performance</t>
+  </si>
+  <si>
+    <t>EXP11.txt</t>
+  </si>
+  <si>
+    <t>Feb. 19, 2017</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 8 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP11.txt</t>
+  </si>
+  <si>
+    <t>LSTM cell, batchsize = 40, two times more updates (40,000 instead of 20,000): To see if LSTM performance improves more.</t>
+  </si>
+  <si>
+    <t>DLT2 / 2</t>
+  </si>
+  <si>
+    <t>EXP12.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justLSTM True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 9 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP12.txt</t>
   </si>
 </sst>
 </file>
@@ -669,11 +693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1069,53 @@
         <v>70</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="1">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experiment in issue #19 done, not concluded though. Kicking off another experiment to confirm a bug.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Experiment description</t>
   </si>
@@ -298,12 +298,64 @@
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justLSTM True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 9 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP12.txt</t>
   </si>
+  <si>
+    <t>Feb. 21, 2017</t>
+  </si>
+  <si>
+    <t>36 hr</t>
+  </si>
+  <si>
+    <t>37 hr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Done! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[buggy]</t>
+    </r>
+  </si>
+  <si>
+    <t>0.5650 / 0.6707 / 3.548</t>
+  </si>
+  <si>
+    <t>0.6323 / 0.7717 / 1.902</t>
+  </si>
+  <si>
+    <t>0.7340 / 0.8672 / 1.091</t>
+  </si>
+  <si>
+    <t>0.5727 / 0.6958 / 3.692</t>
+  </si>
+  <si>
+    <t>model is overfitting!</t>
+  </si>
+  <si>
+    <t>After step 29,000 learning curves are 
+buggy, e.g., loss is NaN! Needs debugging, working on it. Reported results are the results after 29,000 updates right before the bug.</t>
+  </si>
+  <si>
+    <t>Repeating Experiment run_id 8 to confirm if the bug is repeatable.</t>
+  </si>
+  <si>
+    <t>EXP13.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 10 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP13.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,8 +369,15 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -379,6 +444,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,11 +768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,8 +1166,23 @@
       <c r="F13" s="1">
         <v>0</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="L13" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1114,8 +1204,49 @@
       <c r="F14" s="1">
         <v>3</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="L14" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="9">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A couple of experiments for debugging.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>Experiment description</t>
   </si>
@@ -342,13 +342,40 @@
 buggy, e.g., loss is NaN! Needs debugging, working on it. Reported results are the results after 29,000 updates right before the bug.</t>
   </si>
   <si>
-    <t>Repeating Experiment run_id 8 to confirm if the bug is repeatable.</t>
-  </si>
-  <si>
     <t>EXP13.txt</t>
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 10 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP13.txt</t>
+  </si>
+  <si>
+    <t>Feb. 23, 2017</t>
+  </si>
+  <si>
+    <t>81hr</t>
+  </si>
+  <si>
+    <t>Just compare the time of this experiment 
+with that of experiment "EXP10.txt" (row 12)! 
+They are exactly the same experiment but 
+DLT1 is busier and it takes much longer.</t>
+  </si>
+  <si>
+    <t>0.6808 / 0.8232 / 1.515</t>
+  </si>
+  <si>
+    <t>0.6062 / 0.7041 / 3.424</t>
+  </si>
+  <si>
+    <t>Repeating Experiment run_id 8 on DLT1 to confirm if the bug is repeatable.</t>
+  </si>
+  <si>
+    <t>EXP14.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --num_steps 40000 --num_epochs 24 --batch_size 40 --run_id 11 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP14.txt</t>
+  </si>
+  <si>
+    <t>Repeating Experiment run_id 8 on another GPU on DLT2 to confirm if the bug is repeatable.</t>
   </si>
 </sst>
 </file>
@@ -768,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1116,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1107,6 +1134,21 @@
       </c>
       <c r="F11" s="6">
         <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>57</v>
@@ -1225,16 +1267,16 @@
     </row>
     <row r="15" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="9">
         <v>10</v>
@@ -1246,7 +1288,33 @@
         <v>90</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>81</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="9">
+        <v>11</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One more experiment for debugging.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
   <si>
     <t>Experiment description</t>
   </si>
@@ -377,12 +377,24 @@
   <si>
     <t>Repeating Experiment run_id 8 on another GPU on DLT2 to confirm if the bug is repeatable.</t>
   </si>
+  <si>
+    <t>EXP15.txt</t>
+  </si>
+  <si>
+    <t>DLT2 / 1</t>
+  </si>
+  <si>
+    <t>Repeating "EXP11.txt" resuming from iteration 27,000</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 --num_steps 20000 --run_id 12 --resumeTrain True --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/08/save/basic-27000" |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP15.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +411,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -457,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -479,6 +497,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,11 +816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,6 +1338,30 @@
         <v>93</v>
       </c>
     </row>
+    <row r="17" spans="1:12" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="9">
+        <v>12</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off an experiment for regularization. No visualization yet, just trying to use tonight's time.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="110">
   <si>
     <t>Experiment description</t>
   </si>
@@ -388,6 +388,20 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 --num_steps 20000 --run_id 12 --resumeTrain True --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/08/save/basic-20000" |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP15.txt</t>
+  </si>
+  <si>
+    <t>Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. With regularization. No visualization.</t>
+  </si>
+  <si>
+    <t>DLT2 / 4</t>
+  </si>
+  <si>
+    <t>EXP16.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 TPRregularizer1 True --run_id 13 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP16.txt</t>
   </si>
 </sst>
 </file>
@@ -422,7 +436,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +458,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -502,6 +522,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,6 +1387,29 @@
         <v>93</v>
       </c>
     </row>
+    <row r="18" spans="1:12" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="13">
+        <v>13</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="14">
+        <v>42796</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Regularization experiment (run_id_13) concluded.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <t>Experiment description</t>
   </si>
@@ -402,6 +402,21 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 TPRregularizer1 True --run_id 13 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP16.txt</t>
+  </si>
+  <si>
+    <t>13hr</t>
+  </si>
+  <si>
+    <t>No significant improvement in performance compared to no regularization case</t>
+  </si>
+  <si>
+    <t>Bug happened but not repeated at the same iteration.</t>
+  </si>
+  <si>
+    <t>0.5785 / 0.7325 / 2.209</t>
+  </si>
+  <si>
+    <t>0.5477 / 0.6658 / 3.43</t>
   </si>
 </sst>
 </file>
@@ -495,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -516,9 +531,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -844,8 +856,8 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>101</v>
       </c>
@@ -1330,14 +1342,17 @@
       <c r="F15" s="9">
         <v>0</v>
       </c>
+      <c r="G15" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="K15" s="10" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>98</v>
       </c>
@@ -1356,8 +1371,11 @@
       <c r="F16" s="9">
         <v>1</v>
       </c>
+      <c r="G16" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="K16" s="10" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>93</v>
@@ -1382,31 +1400,51 @@
       <c r="F17" s="9">
         <v>3</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="G17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>112</v>
+      </c>
       <c r="L17" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>13</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <v>0</v>
       </c>
-      <c r="L18" s="14">
+      <c r="G18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="13">
         <v>42796</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kicked off an experiment with the new TPRregularization branch.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="145">
   <si>
     <t>Experiment description</t>
   </si>
@@ -418,12 +418,202 @@
   <si>
     <t>0.5477 / 0.6658 / 3.43</t>
   </si>
+  <si>
+    <t>The same as run_id 13 but with 40,000 iterations to see if the bug repeats with regularization.</t>
+  </si>
+  <si>
+    <t>EXP17.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 --num_steps 40000 TPRregularizer1 True --run_id 14 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP17.txt</t>
+  </si>
+  <si>
+    <t>Good news! No bug with Regularization!</t>
+  </si>
+  <si>
+    <t>0.6597 / 0.7978 / 1.63</t>
+  </si>
+  <si>
+    <t>0.5615 / 0.6687 / 3.624</t>
+  </si>
+  <si>
+    <t>28hr</t>
+  </si>
+  <si>
+    <t>To make sure run_id 14 is repeatable with no bug</t>
+  </si>
+  <si>
+    <t>EXP18.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --TPRLSTMCell False --justTPR True --batch_size 40 --num_steps 40000 TPRregularizer1 True --run_id 15 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP18.txt</t>
+  </si>
+  <si>
+    <t>Bug happens after 32K step. Maybe it is something related to our TPR formulation.</t>
+  </si>
+  <si>
+    <t>0.6217 / 0.765 / 1.835</t>
+  </si>
+  <si>
+    <t>0.5655 / 0.6656 / 3.491</t>
+  </si>
+  <si>
+    <t>30hr</t>
+  </si>
+  <si>
+    <t>DLDGX / 4</t>
+  </si>
+  <si>
+    <t>EXP19.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --batch_size 40 --vis True --run_id 16 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP19.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>problematic.</t>
+  </si>
+  <si>
+    <t>EXP20.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. [resolved the problem with config.vis]</t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --batch_size 40 --TPRvis False --run_id 17 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP20.txt</t>
+  </si>
+  <si>
+    <t>DLDGX / 3</t>
+  </si>
+  <si>
+    <t>EXP21.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --batch_size 40 --TPRvis True --run_id 18 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP21.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. [in QA_TPR_for_Run_new]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. [Resuming from latest successful commit, running from QA_TPR_for_Run_new2]</t>
+    </r>
+  </si>
+  <si>
+    <t>DLDGX / 5</t>
+  </si>
+  <si>
+    <t>EXP22.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --batch_size 40 --TPRvis True --run_id 19 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP22.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +636,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,11 +1051,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1646,180 @@
         <v>42796</v>
       </c>
     </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="12">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L19" s="13">
+        <v>42802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="12">
+        <v>15</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" s="13">
+        <v>42802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="12">
+        <v>16</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L21" s="13">
+        <v>42806</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="12">
+        <v>17</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="12">
+        <v>18</v>
+      </c>
+      <c r="F23" s="12">
+        <v>3</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="12">
+        <v>19</v>
+      </c>
+      <c r="F24" s="12">
+        <v>2</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off a set of experiments for regularized TPR with different weights [orange color in table]
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="179">
   <si>
     <t>Experiment description</t>
   </si>
@@ -823,6 +823,326 @@
   </si>
   <si>
     <t>Not problematic.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP27.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 False --TPRvis False --batch_size 40 --run_id 24 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP27.txt</t>
+  </si>
+  <si>
+    <t>EXP28.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis False --batch_size 40 --run_id 25 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP28.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP29.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --batch_size 40 --run_id 26 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP29.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP30.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.1 --cR 0.1 --batch_size 40 --run_id 27 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP30.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP31.txt</t>
+  </si>
+  <si>
+    <t>DLDGX / 6</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.01 --cR 0.01 --batch_size 40 --run_id 28 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP31.txt</t>
   </si>
 </sst>
 </file>
@@ -865,7 +1185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,6 +1213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -953,6 +1279,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1267,11 +1598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,6 +2497,116 @@
         <v>42807</v>
       </c>
     </row>
+    <row r="29" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="15">
+        <v>24</v>
+      </c>
+      <c r="F29" s="15">
+        <v>2</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="16"/>
+    </row>
+    <row r="30" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" s="15">
+        <v>25</v>
+      </c>
+      <c r="F30" s="15">
+        <v>3</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="16"/>
+    </row>
+    <row r="31" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" s="15">
+        <v>26</v>
+      </c>
+      <c r="F31" s="15">
+        <v>4</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="16"/>
+    </row>
+    <row r="32" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="15">
+        <v>27</v>
+      </c>
+      <c r="F32" s="15">
+        <v>5</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="16"/>
+    </row>
+    <row r="33" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="15">
+        <v>28</v>
+      </c>
+      <c r="F33" s="15">
+        <v>1</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="16"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
An experiment for regularized TPR with regularization weight = 0.00001.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="183">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1143,6 +1143,85 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.0 --cR 0.0 --batch_size 40 --run_id 28 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP31.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Resuming from latest successful commit, running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP32.txt</t>
+  </si>
+  <si>
+    <t>DLDGX / 7</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP32.txt</t>
   </si>
 </sst>
 </file>
@@ -1598,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -2607,6 +2686,28 @@
       <c r="K33" s="14"/>
       <c r="L33" s="16"/>
     </row>
+    <row r="34" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="15">
+        <v>29</v>
+      </c>
+      <c r="F34" s="15">
+        <v>0</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="16"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Experiments for regularized TPR with different regularization weights.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="201">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1453,6 +1453,31 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.01 --cR 0.01 --batch_size 40 --run_id 32 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP35.txt</t>
+  </si>
+  <si>
+    <t>DLDGX shut down in 
+the middle of experiment :( Running this on DLT1.</t>
+  </si>
+  <si>
+    <t>EXP36.txt</t>
+  </si>
+  <si>
+    <t>DLT1 / 1</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.0001 --cR 0.0001 --batch_size 40 --run_id 33 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP36.txt</t>
+  </si>
+  <si>
+    <t>EXP37.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.001 --cR 0.001 --batch_size 40 --run_id 34 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP37.txt</t>
+  </si>
+  <si>
+    <t>EXP38.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.01 --cR 0.01 --batch_size 40 --run_id 35 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP38.txt</t>
   </si>
 </sst>
 </file>
@@ -1908,11 +1933,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,6 +3001,9 @@
       <c r="F35" s="15">
         <v>2</v>
       </c>
+      <c r="G35" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="K35" s="14"/>
       <c r="L35" s="16"/>
     </row>
@@ -2998,6 +3026,9 @@
       <c r="F36" s="15">
         <v>3</v>
       </c>
+      <c r="G36" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="K36" s="14"/>
       <c r="L36" s="16"/>
     </row>
@@ -3020,8 +3051,80 @@
       <c r="F37" s="15">
         <v>4</v>
       </c>
+      <c r="G37" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="K37" s="14"/>
       <c r="L37" s="16"/>
+    </row>
+    <row r="38" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E38" s="15">
+        <v>33</v>
+      </c>
+      <c r="F38" s="15">
+        <v>2</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="16"/>
+    </row>
+    <row r="39" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" s="15">
+        <v>34</v>
+      </c>
+      <c r="F39" s="15">
+        <v>3</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="16"/>
+    </row>
+    <row r="40" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="15">
+        <v>35</v>
+      </c>
+      <c r="F40" s="15">
+        <v>4</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Experiments for regularized TPR with different nRoles and nSymbols.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="210">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1478,6 +1478,234 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.01 --cR 0.01 --batch_size 40 --run_id 35 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP38.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=50, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP39.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 50 --nSymbols 100 --batch_size 40 --run_id 36 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP39.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=20, nSymbols=150</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP40.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 150 --batch_size 40 --run_id 37 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP40.txt</t>
+  </si>
+  <si>
+    <t>EXP41.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=50, nSymbols=150</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from QA_TPR_for_Run_TPRregularizationFinal]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 50 --nSymbols 150 --batch_size 40 --run_id 38 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP41.txt</t>
   </si>
 </sst>
 </file>
@@ -1933,11 +2161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3076,7 +3304,9 @@
       <c r="F38" s="15">
         <v>2</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="K38" s="14"/>
       <c r="L38" s="16"/>
     </row>
@@ -3099,7 +3329,9 @@
       <c r="F39" s="15">
         <v>3</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="K39" s="14"/>
       <c r="L39" s="16"/>
     </row>
@@ -3122,9 +3354,77 @@
       <c r="F40" s="15">
         <v>4</v>
       </c>
-      <c r="G40" s="14"/>
+      <c r="G40" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="K40" s="14"/>
       <c r="L40" s="16"/>
+    </row>
+    <row r="41" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E41" s="12">
+        <v>36</v>
+      </c>
+      <c r="F41" s="12">
+        <v>2</v>
+      </c>
+      <c r="K41" s="11"/>
+      <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42" s="12">
+        <v>37</v>
+      </c>
+      <c r="F42" s="12">
+        <v>3</v>
+      </c>
+      <c r="K42" s="11"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="12">
+        <v>38</v>
+      </c>
+      <c r="F43" s="12">
+        <v>4</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Repeating experiment for regularized TPR from new master branch.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="213">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1706,6 +1706,82 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 50 --nSymbols 150 --batch_size 40 --run_id 38 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP41.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Repeating experiment run_id 29 from new master branch for repeatability purposes, running from QA_TPR_for_Run]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP42.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 39 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP42.txt</t>
   </si>
 </sst>
 </file>
@@ -2161,11 +2237,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3435,6 +3511,30 @@
       <c r="K43" s="11"/>
       <c r="L43" s="13"/>
     </row>
+    <row r="44" spans="1:12" s="15" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" s="15">
+        <v>39</v>
+      </c>
+      <c r="F44" s="15">
+        <v>2</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="16">
+        <v>42815</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Concluded different number of roles/symbols experiment.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="219">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1782,6 +1782,91 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 39 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP42.txt</t>
+  </si>
+  <si>
+    <t>EXP43.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --JustLastIterVis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 40 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP43.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Just visualize activations of last iteration, running from QA_TPR_for_Run]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP44.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --JustLastIterVis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 41 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP44.txt</t>
+  </si>
+  <si>
+    <t>The same as above [run_id 40] but on DLDGX because DLT1 is slow and I might not get the results for tomorrow meeting.</t>
   </si>
 </sst>
 </file>
@@ -2237,11 +2322,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,6 +3620,57 @@
         <v>42815</v>
       </c>
     </row>
+    <row r="45" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="15">
+        <v>40</v>
+      </c>
+      <c r="F45" s="15">
+        <v>3</v>
+      </c>
+      <c r="K45" s="14"/>
+      <c r="L45" s="16">
+        <v>42815</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="15">
+        <v>41</v>
+      </c>
+      <c r="F46" s="15">
+        <v>2</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="16">
+        <v>42815</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
different nRoles / nSymbols experiment concluded.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="219">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1782,6 +1782,91 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 39 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP42.txt</t>
+  </si>
+  <si>
+    <t>EXP43.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --JustLastIterVis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 40 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP43.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Just visualize activations of last iteration, running from QA_TPR_for_Run]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP44.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --JustLastIterVis True --cF 0.00001 --cR 0.00001 --batch_size 40 --run_id 41 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP44.txt</t>
+  </si>
+  <si>
+    <t>The same as above [run_id 40] but on DLDGX because DLT1 is slow and I might not get the results for tomorrow meeting.</t>
   </si>
 </sst>
 </file>
@@ -2237,11 +2322,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,6 +3620,57 @@
         <v>42815</v>
       </c>
     </row>
+    <row r="45" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="15">
+        <v>40</v>
+      </c>
+      <c r="F45" s="15">
+        <v>3</v>
+      </c>
+      <c r="K45" s="14"/>
+      <c r="L45" s="16">
+        <v>42815</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="15">
+        <v>41</v>
+      </c>
+      <c r="F46" s="15">
+        <v>2</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="16">
+        <v>42815</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Visualization of roles / symbols / words assignments for first 15 words in the context side.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -2325,8 +2325,8 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Experiment with 30 Roles submitted to DLT1
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="222">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1867,6 +1867,82 @@
   </si>
   <si>
     <t>The same as above [run_id 40] but on DLDGX because DLT1 is slow and I might not get the results for tomorrow meeting.</t>
+  </si>
+  <si>
+    <t>EXP45.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 30 --nSymbols 100 --batch_size 40 --run_id 42 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP45.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=30, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "TPR_Visualization" ]. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1909,7 +1985,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1946,6 +2022,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1974,7 +2056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2008,6 +2090,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2322,11 +2409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,6 +3758,33 @@
         <v>42815</v>
       </c>
     </row>
+    <row r="47" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E47" s="12">
+        <v>42</v>
+      </c>
+      <c r="F47" s="12">
+        <v>2</v>
+      </c>
+      <c r="K47" s="11"/>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="19"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Write aR/aF of whole test set into an excel file.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="223">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2416,7 +2416,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3780,6 +3780,9 @@
       <c r="F47" s="12">
         <v>2</v>
       </c>
+      <c r="G47" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="K47" s="11"/>
       <c r="L47" s="13"/>
     </row>

</xml_diff>

<commit_message>
Kicked of the experiment for writing aR/aF of whole test set into an excel file for 20 roles and 30 roles.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="231">
   <si>
     <t>Experiment description</t>
   </si>
@@ -1946,6 +1946,76 @@
   </si>
   <si>
     <t>DLT1 / 6</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aR &amp; aF vector to excel for the whole test set, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nRoles=20. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[running from "QA_TPR_for_Run" branch "TPR_Visualization" ]</t>
+    </r>
+  </si>
+  <si>
+    <t>EXP46.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aR &amp; aF vector to excel for the whole test set, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nRoles=30. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[running from "QA_TPR_for_Run" branch "TPR_Visualization" ]</t>
+    </r>
+  </si>
+  <si>
+    <t>EXP47.txt</t>
+  </si>
+  <si>
+    <t>from run_id=29</t>
+  </si>
+  <si>
+    <t>from run_id=42</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --write2csv True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP46.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --write2csv True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 30 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/42/save/basic-20000" --run_id 42 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP47.txt</t>
   </si>
 </sst>
 </file>
@@ -2027,7 +2097,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2412,11 +2482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,7 +2495,7 @@
     <col min="2" max="2" width="27.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="29.5703125" style="3" customWidth="1"/>
@@ -3784,12 +3854,53 @@
         <v>14</v>
       </c>
       <c r="K47" s="11"/>
-      <c r="L47" s="13"/>
-    </row>
-    <row r="48" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="L47" s="13">
+        <v>42828</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F48" s="18">
+        <v>2</v>
+      </c>
       <c r="K48" s="17"/>
       <c r="L48" s="19"/>
+    </row>
+    <row r="49" spans="1:12" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F49" s="18">
+        <v>3</v>
+      </c>
+      <c r="K49" s="17"/>
+      <c r="L49" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Concluded the experiment for writing aR/aF of whole test set into an excel file for 20 roles and 30 roles.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="231">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2486,7 +2486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,6 +3877,9 @@
       <c r="F48" s="18">
         <v>2</v>
       </c>
+      <c r="G48" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K48" s="17"/>
       <c r="L48" s="19"/>
     </row>
@@ -3898,6 +3901,9 @@
       </c>
       <c r="F49" s="18">
         <v>3</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="K49" s="17"/>
       <c r="L49" s="19"/>

</xml_diff>

<commit_message>
Kicked off two experiments: nRoels=25 and batchsize=60 [Just TPR for now].
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="238">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2019,6 +2019,137 @@
   </si>
   <si>
     <t>Results successfully repeated.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+batchsize = 40. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With visualizations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With regularization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=25, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP48.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 25 --nSymbols 100 --batch_size 40 --run_id 43 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP48.txt</t>
+  </si>
+  <si>
+    <t>EXP49.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>batchsize = 60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 60 --run_id 44 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP49.txt</t>
   </si>
 </sst>
 </file>
@@ -2485,11 +2616,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3919,6 +4050,50 @@
       <c r="K49" s="17"/>
       <c r="L49" s="19"/>
     </row>
+    <row r="50" spans="1:12" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E50" s="12">
+        <v>43</v>
+      </c>
+      <c r="F50" s="12">
+        <v>2</v>
+      </c>
+      <c r="K50" s="11"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E51" s="12">
+        <v>44</v>
+      </c>
+      <c r="F51" s="12">
+        <v>3</v>
+      </c>
+      <c r="K51" s="11"/>
+      <c r="L51" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off the experiment with Stanford POS tagger on the whole test set!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="241">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2150,6 +2150,38 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 60 --run_id 44 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP49.txt</t>
+  </si>
+  <si>
+    <t>EXP50.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aR &amp; aF vector to excel for the whole test set, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nRoles=20 + Stanford POS Tagger. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[running from "QA_TPR_for_Run" branch "Add_Stanford_POS_Tagger" ]</t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --write2csv True --POStagger True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP50.txt</t>
   </si>
 </sst>
 </file>
@@ -2616,11 +2648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4094,6 +4126,28 @@
       <c r="K51" s="11"/>
       <c r="L51" s="13"/>
     </row>
+    <row r="52" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F52" s="18">
+        <v>2</v>
+      </c>
+      <c r="K52" s="17"/>
+      <c r="L52" s="19"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off one of the DLT1 experiments on DLDGX to get the results faster!
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="245">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2182,6 +2182,18 @@
   </si>
   <si>
     <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --write2csv True --POStagger True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP50.txt</t>
+  </si>
+  <si>
+    <t>The same as run_id 44 but on DLDGX machine which is quite faster.</t>
+  </si>
+  <si>
+    <t>EXP51.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 60 --run_id 45 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP51.txt</t>
+  </si>
+  <si>
+    <t>DLDGX / 0</t>
   </si>
 </sst>
 </file>
@@ -2648,11 +2660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4148,6 +4160,28 @@
       <c r="K52" s="17"/>
       <c r="L52" s="19"/>
     </row>
+    <row r="53" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E53" s="12">
+        <v>45</v>
+      </c>
+      <c r="F53" s="12">
+        <v>3</v>
+      </c>
+      <c r="K53" s="11"/>
+      <c r="L53" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Concluded the experiment with batch size=60.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="252">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2184,9 +2184,6 @@
     <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --write2csv True --POStagger True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP50.txt</t>
   </si>
   <si>
-    <t>The same as run_id 44 but on DLDGX machine which is quite faster.</t>
-  </si>
-  <si>
     <t>EXP51.txt</t>
   </si>
   <si>
@@ -2194,6 +2191,171 @@
   </si>
   <si>
     <t>DLDGX / 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>batchsize = 60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. The same as run_id 44 but on DLDGX machine which is quite faster.</t>
+    </r>
+  </si>
+  <si>
+    <t>0.585 / 0.731 / 2.267</t>
+  </si>
+  <si>
+    <t>0.56 / 0.657 / 3.5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.62 / 0.768 / 1.86
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.585 / 0.731 / 2.267  
+[Bsize=40, run_id 29]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.584 / 0.692 / 3.28
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.56 / 0.657 / 3.5
+[Bsize=40, run_id 29]</t>
+    </r>
+  </si>
+  <si>
+    <t>EXP52.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just TPR no LSTM in 
+phrase embedding layer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>batchsize = 60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>num_steps=60,000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 60 --num_steps 60000 --run_id 46 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP52.txt</t>
   </si>
 </sst>
 </file>
@@ -2660,11 +2822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,6 +3868,12 @@
       <c r="G34" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="H34" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>246</v>
+      </c>
       <c r="K34" s="14"/>
       <c r="L34" s="16"/>
     </row>
@@ -4160,18 +4328,18 @@
       <c r="K52" s="17"/>
       <c r="L52" s="19"/>
     </row>
-    <row r="53" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>242</v>
       </c>
       <c r="E53" s="12">
         <v>45</v>
@@ -4179,8 +4347,41 @@
       <c r="F53" s="12">
         <v>3</v>
       </c>
+      <c r="G53" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>248</v>
+      </c>
       <c r="K53" s="11"/>
       <c r="L53" s="13"/>
+    </row>
+    <row r="54" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="E54" s="12">
+        <v>46</v>
+      </c>
+      <c r="F54" s="12">
+        <v>2</v>
+      </c>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Kicked off the experiment for Regularized TPR concatenated with LSTM. Please note that here both cells are independent and their outputs are concatenated. The goal is to see if we can observe the same interpretive behaviour in this combined system.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="256">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2356,6 +2356,61 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 60 --num_steps 60000 --run_id 46 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP52.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00001. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP53.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00001 --cR 0.00001 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 47 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP53.txt</t>
+  </si>
+  <si>
+    <t>batchsize=40 is used because of memory limitation when using batchsize=60.</t>
   </si>
 </sst>
 </file>
@@ -2822,11 +2877,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4383,6 +4438,32 @@
       <c r="K54" s="11"/>
       <c r="L54" s="13"/>
     </row>
+    <row r="55" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="E55" s="12">
+        <v>47</v>
+      </c>
+      <c r="F55" s="12">
+        <v>3</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="K55" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L55" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off the experiment for TPR concatenated with LSTM cell.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="256">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2880,8 +2880,8 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,6 +4358,9 @@
       <c r="F51" s="12">
         <v>3</v>
       </c>
+      <c r="G51" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="K51" s="11"/>
       <c r="L51" s="13"/>
     </row>
@@ -4379,6 +4382,9 @@
       </c>
       <c r="F52" s="18">
         <v>2</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="K52" s="17"/>
       <c r="L52" s="19"/>

</xml_diff>

<commit_message>
Kicked off some experiments with different regularization terms for both just TPR and TPR-LSTM system.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="269">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2411,6 +2411,218 @@
   </si>
   <si>
     <t>batchsize=40 is used because of memory limitation when using batchsize=60.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00005. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP54.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00005 --cR 0.00005 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 48 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP54.txt</t>
+  </si>
+  <si>
+    <t>EXP55.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00003 --cR 0.00006 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 49 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP55.txt</t>
+  </si>
+  <si>
+    <t>EXP56.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>just TPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00005. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00005 --cR 0.00005 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 50 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP56.txt</t>
+  </si>
+  <si>
+    <t>EXP57.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00003 --cR 0.00006 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 51 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP57.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights: cF=0.00003, cR=0.00006. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>just TPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights: cF=0.00003, cR=0.00006. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>Done but not 
+analyzed completly yet.</t>
   </si>
 </sst>
 </file>
@@ -2453,7 +2665,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2496,6 +2708,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2524,7 +2742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2563,6 +2781,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2877,11 +3103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4336,6 +4562,9 @@
       <c r="F50" s="12">
         <v>2</v>
       </c>
+      <c r="G50" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="K50" s="11"/>
       <c r="L50" s="13"/>
     </row>
@@ -4438,6 +4667,9 @@
       </c>
       <c r="F54" s="12">
         <v>2</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
@@ -4463,12 +4695,111 @@
       <c r="F55" s="12">
         <v>3</v>
       </c>
+      <c r="G55" s="23" t="s">
+        <v>268</v>
+      </c>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="K55" s="11" t="s">
         <v>255</v>
       </c>
       <c r="L55" s="13"/>
+    </row>
+    <row r="56" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" s="21">
+        <v>48</v>
+      </c>
+      <c r="F56" s="21">
+        <v>2</v>
+      </c>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="22"/>
+    </row>
+    <row r="57" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="E57" s="21">
+        <v>49</v>
+      </c>
+      <c r="F57" s="21">
+        <v>3</v>
+      </c>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="22"/>
+    </row>
+    <row r="58" spans="1:12" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E58" s="21">
+        <v>50</v>
+      </c>
+      <c r="F58" s="21">
+        <v>4</v>
+      </c>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="22"/>
+    </row>
+    <row r="59" spans="1:12" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="E59" s="21">
+        <v>51</v>
+      </c>
+      <c r="F59" s="21">
+        <v>5</v>
+      </c>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Concluded & analyzed the experiments 47, 48, 49, 50 and 51.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="268">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2619,10 +2619,6 @@
       </rPr>
       <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
     </r>
-  </si>
-  <si>
-    <t>Done but not 
-analyzed completly yet.</t>
   </si>
 </sst>
 </file>
@@ -2786,7 +2782,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3106,8 +3102,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,7 +4692,7 @@
         <v>3</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>268</v>
+        <v>14</v>
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
@@ -4724,6 +4720,9 @@
       <c r="F56" s="21">
         <v>2</v>
       </c>
+      <c r="G56" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
       <c r="K56" s="20"/>
@@ -4748,6 +4747,9 @@
       <c r="F57" s="21">
         <v>3</v>
       </c>
+      <c r="G57" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="K57" s="20"/>
@@ -4772,6 +4774,9 @@
       <c r="F58" s="21">
         <v>4</v>
       </c>
+      <c r="G58" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
       <c r="K58" s="20"/>
@@ -4795,6 +4800,9 @@
       </c>
       <c r="F59" s="21">
         <v>5</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>

</xml_diff>

<commit_message>
Kicked off the experiments for trained TPR-LSTM2CSV and TPR-LSTM with 60,000 updates.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="275">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2619,6 +2619,114 @@
       </rPr>
       <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aR &amp; aF vector to excel for the whole test set, nRoles=20, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR-LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cR=0.00005, cF=0.00005. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[running from "QA_TPR_for_Run" branch "master" ]</t>
+    </r>
+  </si>
+  <si>
+    <t>from run_id=48</t>
+  </si>
+  <si>
+    <t>EXP58.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --LSTMandTPR True --TPRregularizer1 True --TPRvis True --write2csv True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/48/save/basic-20000" --run_id 48 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP58.txt</t>
+  </si>
+  <si>
+    <t>EXP59.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00005. num_steps=60,000,  nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True num_steps=60000 --cF 0.00005 --cR 0.00005 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 52 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP59.txt</t>
   </si>
 </sst>
 </file>
@@ -3099,11 +3207,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4809,6 +4917,52 @@
       <c r="K59" s="20"/>
       <c r="L59" s="22"/>
     </row>
+    <row r="60" spans="1:12" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="F60" s="18">
+        <v>2</v>
+      </c>
+      <c r="K60" s="17"/>
+      <c r="L60" s="19"/>
+    </row>
+    <row r="61" spans="1:12" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="E61" s="21">
+        <v>52</v>
+      </c>
+      <c r="F61" s="21">
+        <v>3</v>
+      </c>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="22"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kicked off some hyper-param search experiments.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="284">
   <si>
     <t>Experiment description</t>
   </si>
@@ -2727,6 +2727,183 @@
   </si>
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --num_steps=60000 --cF 0.00005 --cR 0.00005 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 52 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP59.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00002. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP60.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00002 --cR 0.00002 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 53 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP60.txt</t>
+  </si>
+  <si>
+    <t>EXP61.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+batchsize = 40. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00003. nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00003 --cR 0.00003 --nRoles 20 --nSymbols 100 --batch_size 40 --run_id 54 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP61.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>batchsize = 60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. With visualizations. With regularization. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regularization weights=0.00003. dRoles=5, dSymbols=5, nRoles=20, nSymbols=100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [running from "QA_TPR_for_Run" branch "master" ]. </t>
+    </r>
+  </si>
+  <si>
+    <t>EXP62.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode train --noload --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --TPRvis True --cF 0.00003 --cR 0.00003 --nRoles 20 --nSymbols 100 --dRoles 5 --dSymbols 5 --batch_size 60 --run_id 55 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP62.txt</t>
   </si>
 </sst>
 </file>
@@ -3207,11 +3384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4936,6 +5113,9 @@
       <c r="F60" s="18">
         <v>2</v>
       </c>
+      <c r="G60" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K60" s="17"/>
       <c r="L60" s="19"/>
     </row>
@@ -4962,6 +5142,78 @@
       <c r="I61" s="20"/>
       <c r="K61" s="20"/>
       <c r="L61" s="22"/>
+    </row>
+    <row r="62" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E62" s="21">
+        <v>53</v>
+      </c>
+      <c r="F62" s="21">
+        <v>2</v>
+      </c>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="22"/>
+    </row>
+    <row r="63" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="E63" s="21">
+        <v>54</v>
+      </c>
+      <c r="F63" s="21">
+        <v>4</v>
+      </c>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="22"/>
+    </row>
+    <row r="64" spans="1:12" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="E64" s="21">
+        <v>55</v>
+      </c>
+      <c r="F64" s="21">
+        <v>5</v>
+      </c>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Concluded the experiments 56 and 57. Now we have a TPR-LSTM model that can achieve very close accuracy and F1 score to those reported in the paper.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="306">
   <si>
     <t>Experiment description</t>
   </si>
@@ -3186,12 +3186,97 @@
   <si>
     <t>python -m basic.cli --mode train --noload --len_opt --cluster --justTPR True --TPRregularizer1 True --TPRvis True --cF 0.00003 --cR 0.00003 --nRoles 20 --nSymbols 100 --dRoles 15 --dSymbols 15 --batch_size 60 --num_steps 40000 --run_id 59 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP66.txt</t>
   </si>
+  <si>
+    <t>test set result [using official SQUAD evaluator]
+accuracy / F1 / loss</t>
+  </si>
+  <si>
+    <t>[after 40,000 updates]
+0.796 / 0.909 / 0.756</t>
+  </si>
+  <si>
+    <t>[after 40,000 updates. The best results observed at 20,000-th update]
+step 20,000:
+0.628 / 0.735 / 3.08
+step 40,000:
+0.606 / 0.726 / 3.95 [overfitting]</t>
+  </si>
+  <si>
+    <t>[test results reported for the model at 20,000-th update]
+67.11 / 76.8 / -</t>
+  </si>
+  <si>
+    <t>[after 40,000 updates]
+0.782 / 0.900 / 0.835</t>
+  </si>
+  <si>
+    <t>[after 40,000 updates. The best results observed at 22,000-th update]
+step 22,000:
+0.637 / 0.740 / 3.27
+step 40,000:
+0.603 / 0.719 / 3.87 [overfitting]</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --len_opt --cluster --justLSTM True --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/57/save/basic-20000" --batch_size 60 --run_id 57</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>command in terminal to run test.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">After this the following should be run to call the official SQUAD evaluator:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>python squad/evaluate-v1.1.py $HOME/data/squad/dev-v1.1.json out/basic/&lt;MODEL_NUMBER&gt;/answer/test-&lt;UPDATE_NUMBER&gt;.json</t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --len_opt --cluster --LSTMandTPR True --TPRregularizer1 True --dRoles 9 --dSymbols 9 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/56/save/basic-22000" --batch_size 60 --run_id 56</t>
+  </si>
+  <si>
+    <t>[test results reported for the model at 22,000-th update]
+67.07 / 76.52</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3222,6 +3307,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3304,7 +3411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3352,6 +3459,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3666,69 +3777,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="29.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="38.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="11" width="27.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="38.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3748,7 +3865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3768,7 +3885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -3796,17 +3913,17 @@
       <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -3834,14 +3951,14 @@
       <c r="I6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -3869,14 +3986,14 @@
       <c r="I7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3904,17 +4021,17 @@
       <c r="I8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -3942,14 +4059,14 @@
       <c r="I9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -3977,17 +4094,17 @@
       <c r="I10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -4015,17 +4132,17 @@
       <c r="I11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="N11" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
@@ -4053,14 +4170,14 @@
       <c r="I12" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="L12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="N12" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>73</v>
       </c>
@@ -4088,17 +4205,17 @@
       <c r="I13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="M13" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>77</v>
       </c>
@@ -4126,17 +4243,17 @@
       <c r="I14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>101</v>
       </c>
@@ -4158,14 +4275,14 @@
       <c r="G15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="N15" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>98</v>
       </c>
@@ -4187,14 +4304,14 @@
       <c r="G16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="M16" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="N16" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>104</v>
       </c>
@@ -4216,14 +4333,14 @@
       <c r="G17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="M17" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>106</v>
       </c>
@@ -4251,17 +4368,17 @@
       <c r="I18" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="L18" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="M18" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="L18" s="13">
+      <c r="N18" s="13">
         <v>42796</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>115</v>
       </c>
@@ -4289,17 +4406,17 @@
       <c r="I19" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="L19" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="M19" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="L19" s="13">
+      <c r="N19" s="13">
         <v>42802</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>122</v>
       </c>
@@ -4327,17 +4444,17 @@
       <c r="I20" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="M20" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="L20" s="13">
+      <c r="N20" s="13">
         <v>42802</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>132</v>
       </c>
@@ -4359,17 +4476,17 @@
       <c r="G21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="L21" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="M21" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="L21" s="13">
+      <c r="N21" s="13">
         <v>42806</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>135</v>
       </c>
@@ -4391,14 +4508,14 @@
       <c r="G22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="M22" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="L22" s="13">
+      <c r="N22" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>140</v>
       </c>
@@ -4417,10 +4534,10 @@
       <c r="F23" s="12">
         <v>3</v>
       </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="M23" s="11"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>141</v>
       </c>
@@ -4442,14 +4559,14 @@
       <c r="G24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="M24" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L24" s="13">
+      <c r="N24" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>145</v>
       </c>
@@ -4471,14 +4588,14 @@
       <c r="G25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="M25" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="L25" s="13">
+      <c r="N25" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>148</v>
       </c>
@@ -4500,14 +4617,14 @@
       <c r="G26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="M26" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="L26" s="13">
+      <c r="N26" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="12" customFormat="1" ht="225" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>155</v>
       </c>
@@ -4529,14 +4646,14 @@
       <c r="G27" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="M27" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="L27" s="13">
+      <c r="N27" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="12" customFormat="1" ht="270" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>161</v>
       </c>
@@ -4558,14 +4675,14 @@
       <c r="G28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="M28" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="L28" s="13">
+      <c r="N28" s="13">
         <v>42807</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>163</v>
       </c>
@@ -4587,10 +4704,10 @@
       <c r="G29" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="16"/>
-    </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="M29" s="14"/>
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="1:14" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>167</v>
       </c>
@@ -4612,10 +4729,10 @@
       <c r="G30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="16"/>
-    </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="M30" s="14"/>
+      <c r="N30" s="16"/>
+    </row>
+    <row r="31" spans="1:14" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>169</v>
       </c>
@@ -4637,10 +4754,10 @@
       <c r="G31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="16"/>
-    </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M31" s="14"/>
+      <c r="N31" s="16"/>
+    </row>
+    <row r="32" spans="1:14" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>172</v>
       </c>
@@ -4662,10 +4779,10 @@
       <c r="G32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="16"/>
-    </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M32" s="14"/>
+      <c r="N32" s="16"/>
+    </row>
+    <row r="33" spans="1:14" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>177</v>
       </c>
@@ -4687,10 +4804,10 @@
       <c r="G33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="16"/>
-    </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M33" s="14"/>
+      <c r="N33" s="16"/>
+    </row>
+    <row r="34" spans="1:14" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>179</v>
       </c>
@@ -4718,10 +4835,10 @@
       <c r="I34" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="16"/>
-    </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M34" s="14"/>
+      <c r="N34" s="16"/>
+    </row>
+    <row r="35" spans="1:14" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>183</v>
       </c>
@@ -4743,10 +4860,10 @@
       <c r="G35" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="16"/>
-    </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M35" s="14"/>
+      <c r="N35" s="16"/>
+    </row>
+    <row r="36" spans="1:14" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>187</v>
       </c>
@@ -4768,10 +4885,10 @@
       <c r="G36" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="16"/>
-    </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M36" s="14"/>
+      <c r="N36" s="16"/>
+    </row>
+    <row r="37" spans="1:14" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>190</v>
       </c>
@@ -4793,10 +4910,10 @@
       <c r="G37" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="16"/>
-    </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M37" s="14"/>
+      <c r="N37" s="16"/>
+    </row>
+    <row r="38" spans="1:14" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>183</v>
       </c>
@@ -4818,10 +4935,10 @@
       <c r="G38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="16"/>
-    </row>
-    <row r="39" spans="1:12" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M38" s="14"/>
+      <c r="N38" s="16"/>
+    </row>
+    <row r="39" spans="1:14" s="15" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>187</v>
       </c>
@@ -4843,10 +4960,10 @@
       <c r="G39" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="16"/>
-    </row>
-    <row r="40" spans="1:12" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M39" s="14"/>
+      <c r="N39" s="16"/>
+    </row>
+    <row r="40" spans="1:14" s="15" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>190</v>
       </c>
@@ -4868,10 +4985,10 @@
       <c r="G40" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="16"/>
-    </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M40" s="14"/>
+      <c r="N40" s="16"/>
+    </row>
+    <row r="41" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>201</v>
       </c>
@@ -4893,10 +5010,10 @@
       <c r="G41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="11"/>
-      <c r="L41" s="13"/>
-    </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M41" s="11"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>204</v>
       </c>
@@ -4918,10 +5035,10 @@
       <c r="G42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M42" s="11"/>
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>208</v>
       </c>
@@ -4943,10 +5060,10 @@
       <c r="G43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="13"/>
-    </row>
-    <row r="44" spans="1:12" s="15" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="M43" s="11"/>
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="1:14" s="15" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>210</v>
       </c>
@@ -4968,14 +5085,14 @@
       <c r="G44" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="M44" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="L44" s="16">
+      <c r="N44" s="16">
         <v>42815</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>215</v>
       </c>
@@ -4997,12 +5114,12 @@
       <c r="G45" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="16">
+      <c r="M45" s="14"/>
+      <c r="N45" s="16">
         <v>42815</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>218</v>
       </c>
@@ -5024,12 +5141,12 @@
       <c r="G46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="16">
+      <c r="M46" s="14"/>
+      <c r="N46" s="16">
         <v>42815</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>221</v>
       </c>
@@ -5051,12 +5168,12 @@
       <c r="G47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K47" s="11"/>
-      <c r="L47" s="13">
+      <c r="M47" s="11"/>
+      <c r="N47" s="13">
         <v>42828</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>223</v>
       </c>
@@ -5078,10 +5195,10 @@
       <c r="G48" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="17"/>
-      <c r="L48" s="19"/>
-    </row>
-    <row r="49" spans="1:12" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="M48" s="17"/>
+      <c r="N48" s="19"/>
+    </row>
+    <row r="49" spans="1:14" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>225</v>
       </c>
@@ -5103,10 +5220,10 @@
       <c r="G49" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K49" s="17"/>
-      <c r="L49" s="19"/>
-    </row>
-    <row r="50" spans="1:12" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M49" s="17"/>
+      <c r="N49" s="19"/>
+    </row>
+    <row r="50" spans="1:14" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>232</v>
       </c>
@@ -5128,10 +5245,10 @@
       <c r="G50" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K50" s="11"/>
-      <c r="L50" s="13"/>
-    </row>
-    <row r="51" spans="1:12" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M50" s="11"/>
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="1:14" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>236</v>
       </c>
@@ -5153,10 +5270,10 @@
       <c r="G51" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K51" s="11"/>
-      <c r="L51" s="13"/>
-    </row>
-    <row r="52" spans="1:12" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="M51" s="11"/>
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="1:14" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>239</v>
       </c>
@@ -5178,10 +5295,10 @@
       <c r="G52" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K52" s="17"/>
-      <c r="L52" s="19"/>
-    </row>
-    <row r="53" spans="1:12" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="M52" s="17"/>
+      <c r="N52" s="19"/>
+    </row>
+    <row r="53" spans="1:14" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>244</v>
       </c>
@@ -5209,10 +5326,12 @@
       <c r="I53" s="11" t="s">
         <v>248</v>
       </c>
+      <c r="J53" s="11"/>
       <c r="K53" s="11"/>
-      <c r="L53" s="13"/>
-    </row>
-    <row r="54" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M53" s="11"/>
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>250</v>
       </c>
@@ -5236,10 +5355,12 @@
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
       <c r="K54" s="11"/>
-      <c r="L54" s="13"/>
-    </row>
-    <row r="55" spans="1:12" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M54" s="11"/>
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="1:14" s="12" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>252</v>
       </c>
@@ -5263,12 +5384,14 @@
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
-      <c r="K55" s="11" t="s">
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="M55" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="L55" s="13"/>
-    </row>
-    <row r="56" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="1:14" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>256</v>
       </c>
@@ -5292,10 +5415,12 @@
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
       <c r="K56" s="20"/>
-      <c r="L56" s="22"/>
-    </row>
-    <row r="57" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M56" s="20"/>
+      <c r="N56" s="22"/>
+    </row>
+    <row r="57" spans="1:14" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>266</v>
       </c>
@@ -5319,10 +5444,12 @@
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
       <c r="K57" s="20"/>
-      <c r="L57" s="22"/>
-    </row>
-    <row r="58" spans="1:12" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M57" s="20"/>
+      <c r="N57" s="22"/>
+    </row>
+    <row r="58" spans="1:14" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>262</v>
       </c>
@@ -5346,10 +5473,12 @@
       </c>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
       <c r="K58" s="20"/>
-      <c r="L58" s="22"/>
-    </row>
-    <row r="59" spans="1:12" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="M58" s="20"/>
+      <c r="N58" s="22"/>
+    </row>
+    <row r="59" spans="1:14" s="21" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>267</v>
       </c>
@@ -5373,10 +5502,12 @@
       </c>
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
       <c r="K59" s="20"/>
-      <c r="L59" s="22"/>
-    </row>
-    <row r="60" spans="1:12" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="M59" s="20"/>
+      <c r="N59" s="22"/>
+    </row>
+    <row r="60" spans="1:14" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>268</v>
       </c>
@@ -5398,10 +5529,10 @@
       <c r="G60" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K60" s="17"/>
-      <c r="L60" s="19"/>
-    </row>
-    <row r="61" spans="1:12" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="M60" s="17"/>
+      <c r="N60" s="19"/>
+    </row>
+    <row r="61" spans="1:14" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>273</v>
       </c>
@@ -5422,10 +5553,12 @@
       </c>
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
       <c r="K61" s="20"/>
-      <c r="L61" s="22"/>
-    </row>
-    <row r="62" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M61" s="20"/>
+      <c r="N61" s="22"/>
+    </row>
+    <row r="62" spans="1:14" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>274</v>
       </c>
@@ -5446,10 +5579,12 @@
       </c>
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
       <c r="K62" s="20"/>
-      <c r="L62" s="22"/>
-    </row>
-    <row r="63" spans="1:12" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="M62" s="20"/>
+      <c r="N62" s="22"/>
+    </row>
+    <row r="63" spans="1:14" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>278</v>
       </c>
@@ -5470,10 +5605,12 @@
       </c>
       <c r="H63" s="20"/>
       <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
       <c r="K63" s="20"/>
-      <c r="L63" s="22"/>
-    </row>
-    <row r="64" spans="1:12" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="M63" s="20"/>
+      <c r="N63" s="22"/>
+    </row>
+    <row r="64" spans="1:14" s="21" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>280</v>
       </c>
@@ -5494,10 +5631,12 @@
       </c>
       <c r="H64" s="20"/>
       <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
       <c r="K64" s="20"/>
-      <c r="L64" s="22"/>
-    </row>
-    <row r="65" spans="1:12" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="M64" s="20"/>
+      <c r="N64" s="22"/>
+    </row>
+    <row r="65" spans="1:14" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>285</v>
       </c>
@@ -5516,12 +5655,25 @@
       <c r="F65" s="12">
         <v>2</v>
       </c>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="13"/>
-    </row>
-    <row r="66" spans="1:12" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="G65" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="M65" s="11"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="1:14" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>287</v>
       </c>
@@ -5540,12 +5692,25 @@
       <c r="F66" s="12">
         <v>3</v>
       </c>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="13"/>
-    </row>
-    <row r="67" spans="1:12" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="G66" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="J66" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="K66" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="M66" s="11"/>
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="1:14" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>291</v>
       </c>
@@ -5567,10 +5732,12 @@
       <c r="G67" s="24"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
       <c r="K67" s="11"/>
-      <c r="L67" s="13"/>
-    </row>
-    <row r="68" spans="1:12" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="M67" s="11"/>
+      <c r="N67" s="13"/>
+    </row>
+    <row r="68" spans="1:14" s="12" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>293</v>
       </c>
@@ -5592,8 +5759,10 @@
       <c r="G68" s="24"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
       <c r="K68" s="11"/>
-      <c r="L68" s="13"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Kicked off the experiment to generate excel files including aF and aR vectors for the whole test set for the best model we have so far, run_id 56 (independent TPR-LSTM model).
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="311">
   <si>
     <t>Experiment description</t>
   </si>
@@ -3273,6 +3273,73 @@
   </si>
   <si>
     <t>Did not achieve the same performance as batch size 60 although increased the number of updates significantly.</t>
+  </si>
+  <si>
+    <t>from run_id=56</t>
+  </si>
+  <si>
+    <t>EXP67.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aR &amp; aF vector to excel for the whole test set, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TPR concatenated with LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+phrase embedding layer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, num_steps=40000. With visualizations. With regularization. Regularization weights=0.00003. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dRoles=9, dSymbols=9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, nRoles=20, nSymbols=100 [running from "QA_TPR_for_Run" branch "master" ].</t>
+    </r>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --LSTMandTPR True --TPRregularizer1 True --TPRvis True --write2csv True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --nSymbols 100 --dRoles 9 --dSymbols 9 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/56/save/basic-22000" --run_id 56 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP67.txt</t>
   </si>
 </sst>
 </file>
@@ -3780,11 +3847,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5781,6 +5848,28 @@
       <c r="M68" s="11"/>
       <c r="N68" s="13"/>
     </row>
+    <row r="69" spans="1:14" s="18" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="F69" s="18">
+        <v>2</v>
+      </c>
+      <c r="M69" s="17"/>
+      <c r="N69" s="19"/>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
setting the status of previous experiments.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="311">
   <si>
     <t>Experiment description</t>
   </si>
@@ -5867,6 +5867,9 @@
       <c r="F69" s="18">
         <v>2</v>
       </c>
+      <c r="G69" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="M69" s="17"/>
       <c r="N69" s="19"/>
     </row>

</xml_diff>

<commit_message>
Added the results of official SQUAD test for TPR model to experiments.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="315">
   <si>
     <t>Experiment description</t>
   </si>
@@ -3340,6 +3340,35 @@
   </si>
   <si>
     <t>python -m basic.cli --mode test --LSTMandTPR True --TPRregularizer1 True --TPRvis True --write2csv True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --nSymbols 100 --dRoles 9 --dSymbols 9 --vis True --batch_size 40 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/56/save/basic-22000" --run_id 56 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP67.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --len_opt --cluster --justTPR True --TPRregularizer1 True --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/45/save/basic-20000" --batch_size 60 --run_id 45</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --len_opt --cluster --justTPR True --TPRregularizer1 True --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --batch_size 60 --run_id 29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[test results reported for the model at 20,000-th update]
+65.34 / 74.86 / -
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>63.75 / 73.63 / -
+[Bsize=40, run_id 29]</t>
+    </r>
+  </si>
+  <si>
+    <t>[test results reported for the 
+model at 20,000-th update]
+63.75 / 73.63 / -</t>
   </si>
 </sst>
 </file>
@@ -3850,8 +3879,8 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4905,6 +4934,12 @@
       <c r="I34" s="15" t="s">
         <v>246</v>
       </c>
+      <c r="J34" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>312</v>
+      </c>
       <c r="M34" s="14"/>
       <c r="N34" s="16"/>
     </row>
@@ -5396,8 +5431,12 @@
       <c r="I53" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
+      <c r="J53" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>311</v>
+      </c>
       <c r="M53" s="11"/>
       <c r="N53" s="13"/>
     </row>

</xml_diff>

<commit_message>
F * a_F visualization per word. Not complete yet.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="319">
   <si>
     <t>Experiment description</t>
   </si>
@@ -3369,6 +3369,18 @@
     <t>[test results reported for the 
 model at 20,000-th update]
 63.75 / 73.63 / -</t>
+  </si>
+  <si>
+    <t>The problem here is that we observe a severe localization problem here, i.e., one role responds to all words!</t>
+  </si>
+  <si>
+    <t>EXP68.txt</t>
+  </si>
+  <si>
+    <t>Cosine similarity between F*a_F(t) per word and each column of trained filler matrix F [running from "QA_TPR_for_Run" branch "issue_32" ].</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --Fa_F_vis True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --nSymbols 100 --vis True --batch_size 60 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP68.txt</t>
   </si>
 </sst>
 </file>
@@ -3876,11 +3888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5906,8 +5918,37 @@
       <c r="F69" s="18">
         <v>2</v>
       </c>
-      <c r="M69" s="17"/>
+      <c r="G69" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M69" s="17" t="s">
+        <v>315</v>
+      </c>
       <c r="N69" s="19"/>
+    </row>
+    <row r="70" spans="1:14" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F70" s="18">
+        <v>2</v>
+      </c>
+      <c r="M70" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="N70" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Kicked off the experiment for filler visualizations.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -3901,7 +3901,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
+      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5968,7 +5968,7 @@
         <v>321</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>142</v>
+        <v>195</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>320</v>

</xml_diff>

<commit_message>
Kicked off the experiment for issue 45.
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="325">
   <si>
     <t>Experiment description</t>
   </si>
@@ -3390,6 +3390,15 @@
   </si>
   <si>
     <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --TPRvis True --Fa_F_vis True --which_tensors2vis "fw_u_aR,bw_u_aR,fw_u_aF,bw_u_aF" --nRoles 20 --nSymbols 100 --vis True --batch_size 60 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP69.txt</t>
+  </si>
+  <si>
+    <t>EXP70.txt</t>
+  </si>
+  <si>
+    <t>python -m basic.cli --mode test --justTPR True --TPRregularizer1 True --EMperQ True --nRoles 20 --nSymbols 100 --vis True --batch_size 60 --load_path "/home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/QA_TPR_for_Run/out/basic/29/save/basic-20000" --run_id 29 |&amp; tee /home/hpalangi/QA/TPR_Stuff/Codes/TPR_ver1.0/Log_Files/EXP70.txt</t>
+  </si>
+  <si>
+    <t>Write EM, F1, paragraph, and 3 answers per query for the whole validation set as different columns of an output excel file. [running from "QA_TPR_for_Run" branch "issue_45" ].</t>
   </si>
 </sst>
 </file>
@@ -3531,7 +3540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3583,6 +3592,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3897,11 +3907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5979,8 +5989,33 @@
       <c r="F71" s="18">
         <v>2</v>
       </c>
+      <c r="G71" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="M71" s="17"/>
       <c r="N71" s="19"/>
+    </row>
+    <row r="72" spans="1:14" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F72" s="6">
+        <v>2</v>
+      </c>
+      <c r="M72" s="5"/>
+      <c r="N72" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>